<commit_message>
Refactor: Fix issues in edit API of project and its corresponding modules, remove unnecessary comments, format code, and test edit API functionality
</commit_message>
<xml_diff>
--- a/data/Shirts/Logo Pricing/Upper Back.xlsx
+++ b/data/Shirts/Logo Pricing/Upper Back.xlsx
@@ -497,12 +497,15 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -519,7 +522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -536,7 +539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -553,7 +556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -570,7 +573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -587,7 +590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -604,7 +607,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -621,7 +624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -638,7 +641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -655,7 +658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -672,7 +675,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -689,7 +692,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -706,7 +709,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -723,7 +726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -740,7 +743,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -757,7 +760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -774,7 +777,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -791,7 +794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -808,7 +811,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>

</xml_diff>